<commit_message>
Fix bug Api gmap display icon
</commit_message>
<xml_diff>
--- a/map_project/list.xlsx
+++ b/map_project/list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="343">
   <si>
     <t>Vietnam</t>
   </si>
@@ -1047,6 +1047,15 @@
   </si>
   <si>
     <t>latlng</t>
+  </si>
+  <si>
+    <t>Brussels</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>50.850346, 4.351721</t>
   </si>
 </sst>
 </file>
@@ -1088,18 +1097,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1110,8 +1108,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C155" totalsRowShown="0">
-  <autoFilter ref="A1:C155"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C156" totalsRowShown="0">
+  <autoFilter ref="A1:C156"/>
   <tableColumns count="3">
     <tableColumn id="1" name="country"/>
     <tableColumn id="2" name="city"/>
@@ -1384,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C155"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3102,6 +3100,17 @@
         <v>327</v>
       </c>
     </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>341</v>
+      </c>
+      <c r="B156" t="s">
+        <v>340</v>
+      </c>
+      <c r="C156" t="s">
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:C155">
     <sortCondition ref="A1"/>

</xml_diff>